<commit_message>
mcu bom board and schematic updated !
</commit_message>
<xml_diff>
--- a/BMS_hw/MCU_PCB/PIGGY_MASTER_BOM.xlsx
+++ b/BMS_hw/MCU_PCB/PIGGY_MASTER_BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="123">
   <si>
     <t>Item</t>
   </si>
@@ -51,27 +51,15 @@
     <t>PCB Footprint</t>
   </si>
   <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
     <t>SCH-XXXXX PDF: SPF-XXXXX          Revision: 01</t>
   </si>
   <si>
     <t>0E</t>
   </si>
   <si>
-    <t>10uF</t>
-  </si>
-  <si>
     <t>GF_AFE board Revised: Sunday, OCT 14, 2018</t>
   </si>
   <si>
-    <t>.01uF</t>
-  </si>
-  <si>
-    <t>.1uF</t>
-  </si>
-  <si>
     <t>100R</t>
   </si>
   <si>
@@ -126,12 +114,6 @@
     <t>C22</t>
   </si>
   <si>
-    <t>C17, C18, C19, C20</t>
-  </si>
-  <si>
-    <t>C14, C21</t>
-  </si>
-  <si>
     <t>R5, R6</t>
   </si>
   <si>
@@ -183,44 +165,236 @@
     <t>U$1</t>
   </si>
   <si>
-    <t>1X12X2</t>
-  </si>
-  <si>
-    <t>CHIP-LED0603</t>
-  </si>
-  <si>
-    <t>SOT95P280X135-3N</t>
-  </si>
-  <si>
-    <t>1X15</t>
-  </si>
-  <si>
-    <t>CAPC1005X60N</t>
-  </si>
-  <si>
-    <t>RESC1005X40AN</t>
-  </si>
-  <si>
-    <t>1.4X1.2-4-PAD</t>
-  </si>
-  <si>
-    <t>RESC2012X70N</t>
-  </si>
-  <si>
-    <t>TQFP-64-I/PT</t>
-  </si>
-  <si>
-    <t>SOIC127P600X175-8N</t>
-  </si>
-  <si>
-    <t>SOT162-1</t>
+    <t>SMD 0402</t>
+  </si>
+  <si>
+    <t>RES TKF 10k 1% 1/10W SMD 0402</t>
+  </si>
+  <si>
+    <t>0.1uF/16V</t>
+  </si>
+  <si>
+    <t>10uF/10V</t>
+  </si>
+  <si>
+    <t>AVX Corporation</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 10V X5R 0402</t>
+  </si>
+  <si>
+    <t>0402ZD106MAT2A</t>
+  </si>
+  <si>
+    <t>TDK Corporation</t>
+  </si>
+  <si>
+    <t>FERRITE BEAD 300 OHM 0805 1LN</t>
+  </si>
+  <si>
+    <t>SMD 0805</t>
+  </si>
+  <si>
+    <t>0.01uF/25V</t>
+  </si>
+  <si>
+    <t>CAP CERAMIC 0.01UF 25V X7R 20% P</t>
+  </si>
+  <si>
+    <t>GRM155R71E103MA01D</t>
+  </si>
+  <si>
+    <t>Murata Electronics North America</t>
+  </si>
+  <si>
+    <t>LTST-C190GKT</t>
+  </si>
+  <si>
+    <t>LED GREEN CLEAR CHIP SMD</t>
+  </si>
+  <si>
+    <t>Lite-On Inc.</t>
+  </si>
+  <si>
+    <t>SMD 0603</t>
+  </si>
+  <si>
+    <t>RES SMD 330 OHM 1% 1/10W 0402</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF3300X</t>
+  </si>
+  <si>
+    <t>Panasonic Electronic Components</t>
+  </si>
+  <si>
+    <t>C17, C18, C19, C20,C21,C14</t>
+  </si>
+  <si>
+    <t>Green color</t>
+  </si>
+  <si>
+    <t>NPN Transistor</t>
+  </si>
+  <si>
+    <t>TRANS NPN 40V 0.2A SOT-23</t>
+  </si>
+  <si>
+    <t>ON Semiconductor</t>
+  </si>
+  <si>
+    <t>MMBT3904FSCT-ND</t>
+  </si>
+  <si>
+    <t>SOT-23-3</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 16V Y5V 0402</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>CL05F104ZO5NNNC</t>
+  </si>
+  <si>
+    <t>RES SMD 0 OHM JUMP 1/16W 0402</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>CRCW04020000Z0EDC</t>
+  </si>
+  <si>
+    <t>RES SMD 100 OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>RC0402FR-07100RL</t>
+  </si>
+  <si>
+    <t>120E</t>
+  </si>
+  <si>
+    <t>RES 120 OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RCS1005F121CS</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 0.5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>Susumu</t>
+  </si>
+  <si>
+    <t>RR0510P-102-D</t>
+  </si>
+  <si>
+    <t>CAP CER 20PF 50V C0G/NP0 0402</t>
+  </si>
+  <si>
+    <t>GJM1555C1H200JB01D</t>
+  </si>
+  <si>
+    <t>RES SMD 4.7K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RC0402FR-074K7L</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 16V X5R 0402</t>
+  </si>
+  <si>
+    <t>CL05A475MO5NUNC</t>
+  </si>
+  <si>
+    <t>CAP CER 47PF 50V C0G/NP0 0402</t>
+  </si>
+  <si>
+    <t>04025A470JAT2A</t>
+  </si>
+  <si>
+    <t>60.4E</t>
+  </si>
+  <si>
+    <t>RES SMD 60.4 OHM 1% 1/10W 0402</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF60R4X</t>
+  </si>
+  <si>
+    <t>DGTL ISOLATOR 5KV 2CH CAN 16SO</t>
+  </si>
+  <si>
+    <t>NXP USA Inc.</t>
+  </si>
+  <si>
+    <t>TJA1052IT/5Y</t>
+  </si>
+  <si>
+    <t>IC FLASH 2M SPI 80MHZ 8SOIC</t>
+  </si>
+  <si>
+    <t>Microchip Technology</t>
+  </si>
+  <si>
+    <t>SST25VF020B-80-4I-SAE</t>
+  </si>
+  <si>
+    <t>8-SOIC (0.154", 3.90mm Width)</t>
+  </si>
+  <si>
+    <t>16-SOIC (0.295", 7.50mm Width)</t>
+  </si>
+  <si>
+    <t>IC MCU 32BIT 512KB FLASH 64TQFP</t>
+  </si>
+  <si>
+    <t>64-TQFP</t>
+  </si>
+  <si>
+    <t>CRYSTAL 12.0000MHZ 12PF SMD</t>
+  </si>
+  <si>
+    <t>EPSON</t>
+  </si>
+  <si>
+    <t>FA-238V 12.0000MB-W3</t>
+  </si>
+  <si>
+    <t>4-SMD, No Lead</t>
+  </si>
+  <si>
+    <t>2mm pitch , right angled board to wire 12 pin conn.</t>
+  </si>
+  <si>
+    <t>Through hole, Right Angle</t>
+  </si>
+  <si>
+    <t>Through hole, straight</t>
+  </si>
+  <si>
+    <t>2mm pitch straight board to board 15 pin conn.</t>
+  </si>
+  <si>
+    <t>12 pin</t>
+  </si>
+  <si>
+    <t>15 pin</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +546,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -560,7 +740,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -690,6 +870,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -735,7 +930,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -766,9 +961,15 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1119,11 +1320,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,25 +1335,27 @@
     <col min="5" max="5" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="47.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" style="12" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1182,7 +1385,7 @@
       <c r="I3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="13" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1193,11 +1396,22 @@
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="12"/>
-      <c r="J4" s="8" t="s">
-        <v>55</v>
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1207,11 +1421,22 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="J5" s="8" t="s">
-        <v>56</v>
+        <v>27</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1221,11 +1446,22 @@
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="J6" s="8" t="s">
-        <v>54</v>
+        <v>28</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1235,11 +1471,22 @@
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="J7" s="8" t="s">
-        <v>57</v>
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1249,13 +1496,22 @@
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>58</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1265,13 +1521,22 @@
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>58</v>
+        <v>69</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1281,13 +1546,22 @@
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>58</v>
+        <v>31</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1297,61 +1571,91 @@
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>59</v>
+        <v>32</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>59</v>
+        <v>33</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>59</v>
+        <v>34</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>58</v>
+        <v>35</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1361,47 +1665,70 @@
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="12">
-        <v>120</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="7"/>
+        <v>2</v>
+      </c>
       <c r="D16" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="1">
         <v>2</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="8" t="s">
-        <v>58</v>
+        <v>38</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1410,43 +1737,70 @@
         <v>2</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>59</v>
+        <v>39</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>59</v>
+        <v>40</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>58</v>
+        <v>41</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1455,79 +1809,118 @@
         <v>2</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>58</v>
+        <v>42</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="12">
-        <v>60.4</v>
-      </c>
-      <c r="F22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="8" t="s">
-        <v>59</v>
+        <v>43</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="1">
         <v>1</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>62</v>
+        <v>46</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="J25" s="15" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1536,178 +1929,165 @@
         <v>1</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="H26" s="10"/>
-      <c r="J26" s="8" t="s">
-        <v>63</v>
+        <v>47</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
-      <c r="B27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>64</v>
-      </c>
+      <c r="B27" s="1"/>
+      <c r="D27" s="8"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-      <c r="B28" s="1"/>
-      <c r="D28" s="8"/>
-      <c r="J28" s="8"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="J30" s="8"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="J31" s="8"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="J37" s="8"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E57" s="8"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
-      <c r="E58" s="8"/>
-      <c r="J58" s="8"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E64" s="8"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
-      <c r="E65" s="8"/>
-      <c r="J65" s="8"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1716,6 +2096,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="c4672b8b-43e2-4139-8cd1-27ad03f081e7">
@@ -1731,15 +2120,6 @@
     </dd399bed73eb4e21ba4b4b5eeb50a8b4>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1947,19 +2327,27 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{817A1FC8-D3A3-4B4B-9419-3DB2734E9FAB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFEF643C-744E-47E4-BE01-550303BDE769}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c4672b8b-43e2-4139-8cd1-27ad03f081e7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFEF643C-744E-47E4-BE01-550303BDE769}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{817A1FC8-D3A3-4B4B-9419-3DB2734E9FAB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="1f7e2bd1-5fdf-4d6b-8b99-ef650a991a33"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f8cd1e16-0731-4200-9ee6-df6e2184771e"/>
+    <ds:schemaRef ds:uri="c4672b8b-43e2-4139-8cd1-27ad03f081e7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>